<commit_message>
Starting the Sheet connections
</commit_message>
<xml_diff>
--- a/Electronics/Computations/Book1.xlsx
+++ b/Electronics/Computations/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents2\KiCad\9.0\projects\CM5 Nas\Computations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents2\KiCad\9.0\projects\CM5 Nas\Electronics\Computations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6C7B7B-C28C-4492-9D3A-65ADF4A38331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D60A3EC-C78C-4C2F-A95F-6049C2BCE3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{ABB098FB-230C-42A9-9A75-78B22FD1A26F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ABB098FB-230C-42A9-9A75-78B22FD1A26F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
   <si>
     <t>KSZ9563RNX</t>
   </si>
@@ -72,6 +72,105 @@
   </si>
   <si>
     <t>TPS65251-1RHAR</t>
+  </si>
+  <si>
+    <t>Out</t>
+  </si>
+  <si>
+    <t>PCIE_PWR_EN</t>
+  </si>
+  <si>
+    <t>PCIE_CLK_P</t>
+  </si>
+  <si>
+    <t>PCIE_CLK_N</t>
+  </si>
+  <si>
+    <t>PCIE_TX_P</t>
+  </si>
+  <si>
+    <t>PCIE_TX_N</t>
+  </si>
+  <si>
+    <t>USB3-0-TX_N</t>
+  </si>
+  <si>
+    <t>USB3-0-TX_P</t>
+  </si>
+  <si>
+    <t>PCIE_nRST</t>
+  </si>
+  <si>
+    <t>Detination</t>
+  </si>
+  <si>
+    <t>PG</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>USB3-1-TX_N</t>
+  </si>
+  <si>
+    <t>USB3-1-TX_P</t>
+  </si>
+  <si>
+    <t>USB2_N</t>
+  </si>
+  <si>
+    <t>USB2_P</t>
+  </si>
+  <si>
+    <t>PCIE_nCLKREQ</t>
+  </si>
+  <si>
+    <t>PCIE_nWAKE</t>
+  </si>
+  <si>
+    <t>PCIE_RX_P</t>
+  </si>
+  <si>
+    <t>Origin</t>
+  </si>
+  <si>
+    <t>PCIE_RX_N</t>
+  </si>
+  <si>
+    <t>USB3-0-RX_N</t>
+  </si>
+  <si>
+    <t>USB3-0-RX_P</t>
+  </si>
+  <si>
+    <t>USB3-1-RX_N</t>
+  </si>
+  <si>
+    <t>USB3-1-RX_P</t>
+  </si>
+  <si>
+    <t>GPIO_VREF</t>
+  </si>
+  <si>
+    <t>ID_SC</t>
+  </si>
+  <si>
+    <t>ID_SD</t>
+  </si>
+  <si>
+    <t>CAM_GPIO0</t>
+  </si>
+  <si>
+    <t>CAM_GPIO1</t>
+  </si>
+  <si>
+    <t>SDA0</t>
+  </si>
+  <si>
+    <t>SCL0</t>
+  </si>
+  <si>
+    <t>3V3</t>
   </si>
 </sst>
 </file>
@@ -449,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760FFF89-5808-41D6-9953-2E152F55B009}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q39" sqref="Q39"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="Q34" sqref="Q34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,12 +704,327 @@
         <v>440</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1.2</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+      <c r="F20">
+        <v>4</v>
+      </c>
+      <c r="G20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21" t="s">
+        <v>29</v>
+      </c>
+      <c r="I21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+      <c r="F22">
+        <v>4</v>
+      </c>
+      <c r="G22" t="s">
+        <v>30</v>
+      </c>
+      <c r="I22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23" t="s">
+        <v>32</v>
+      </c>
+      <c r="I23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+      <c r="F24">
+        <v>4</v>
+      </c>
+      <c r="G24" t="s">
+        <v>33</v>
+      </c>
+      <c r="I24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25">
+        <v>9</v>
+      </c>
+      <c r="F25">
+        <v>4</v>
+      </c>
+      <c r="G25" t="s">
+        <v>34</v>
+      </c>
+      <c r="I25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26">
+        <v>9</v>
+      </c>
+      <c r="F26">
+        <v>4</v>
+      </c>
+      <c r="G26" t="s">
+        <v>44</v>
+      </c>
+      <c r="I26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="G27" t="s">
+        <v>35</v>
+      </c>
+      <c r="I27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28">
+        <v>10</v>
+      </c>
+      <c r="F28">
+        <v>4</v>
+      </c>
+      <c r="G28" t="s">
+        <v>36</v>
+      </c>
+      <c r="I28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29">
+        <v>10</v>
+      </c>
+      <c r="F29">
+        <v>4</v>
+      </c>
+      <c r="G29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30">
+        <v>11</v>
+      </c>
+      <c r="F30">
+        <v>4</v>
+      </c>
+      <c r="G30" t="s">
+        <v>38</v>
+      </c>
+      <c r="I30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31">
+        <v>11</v>
+      </c>
+      <c r="F31">
+        <v>4</v>
+      </c>
+      <c r="G31" t="s">
+        <v>39</v>
+      </c>
+      <c r="I31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>4</v>
+      </c>
+      <c r="G32" t="s">
+        <v>40</v>
+      </c>
+      <c r="I32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>4</v>
+      </c>
+      <c r="G33" t="s">
+        <v>41</v>
+      </c>
+      <c r="I33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>4</v>
+      </c>
+      <c r="G34" t="s">
+        <v>43</v>
+      </c>
+      <c r="I34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>4</v>
+      </c>
+      <c r="G35" t="s">
+        <v>42</v>
+      </c>
+      <c r="I35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>4</v>
+      </c>
+      <c r="G36" t="s">
+        <v>44</v>
+      </c>
+      <c r="I36">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>